<commit_message>
New Sheets Alert! participatingAgencies04292025pm.xlsx and pendingAgencies04292025pm.xlsx
</commit_message>
<xml_diff>
--- a/Total pendingAgencies/Total-pendingAgencies04292025pm.xlsx
+++ b/Total pendingAgencies/Total-pendingAgencies04292025pm.xlsx
@@ -446,12 +446,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>STATE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>TYPE</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>STATE</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -469,12 +469,12 @@
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>DELAWARE</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>DELAWARE</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -492,12 +492,12 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -515,12 +515,12 @@
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -538,12 +538,12 @@
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -561,12 +561,12 @@
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -584,12 +584,12 @@
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -607,12 +607,12 @@
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -630,12 +630,12 @@
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -653,12 +653,12 @@
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -676,12 +676,12 @@
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -699,12 +699,12 @@
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -722,12 +722,12 @@
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -745,12 +745,12 @@
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -768,12 +768,12 @@
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -791,12 +791,12 @@
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -814,12 +814,12 @@
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -837,12 +837,12 @@
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -860,12 +860,12 @@
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -883,12 +883,12 @@
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -906,12 +906,12 @@
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -929,12 +929,12 @@
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -952,12 +952,12 @@
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -975,12 +975,12 @@
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -998,12 +998,12 @@
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1021,12 +1021,12 @@
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1044,12 +1044,12 @@
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1067,12 +1067,12 @@
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1090,12 +1090,12 @@
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1113,12 +1113,12 @@
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1136,12 +1136,12 @@
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1159,12 +1159,12 @@
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1182,12 +1182,12 @@
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1205,12 +1205,12 @@
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1228,12 +1228,12 @@
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1251,12 +1251,12 @@
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1274,12 +1274,12 @@
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1297,12 +1297,12 @@
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1320,12 +1320,12 @@
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1343,12 +1343,12 @@
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1366,12 +1366,12 @@
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1389,12 +1389,12 @@
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -1412,12 +1412,12 @@
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1435,12 +1435,12 @@
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1458,12 +1458,12 @@
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1481,12 +1481,12 @@
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1504,12 +1504,12 @@
       <c r="B47" t="inlineStr"/>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1531,12 +1531,12 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1558,12 +1558,12 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1585,12 +1585,12 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1608,12 +1608,12 @@
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1635,12 +1635,12 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1662,12 +1662,12 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1689,12 +1689,12 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1716,12 +1716,12 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>MICHIGAN</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>MICHIGAN</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1739,12 +1739,12 @@
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>MICHIGAN</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>MICHIGAN</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1766,12 +1766,12 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>MISSOURI</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>MISSOURI</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1789,12 +1789,12 @@
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>MISSOURI</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>MISSOURI</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -1816,12 +1816,12 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>MONTANA</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>MONTANA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -1843,12 +1843,12 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>NEBRASKA</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>NEBRASKA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -1870,12 +1870,12 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>NORTH CAROLINA</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>NORTH CAROLINA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -1897,12 +1897,12 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>OKLAHOMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
@@ -1920,12 +1920,12 @@
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
+          <t>OKLAHOMA</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -1943,12 +1943,12 @@
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
+          <t>OKLAHOMA</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D64" t="inlineStr">
-        <is>
-          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -1970,12 +1970,12 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>PENNSYLVANIA</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>PENNSYLVANIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -1997,12 +1997,12 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>PENNSYLVANIA</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>PENNSYLVANIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2024,12 +2024,12 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TENNESSEE</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>TENNESSEE</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2051,12 +2051,12 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
@@ -2078,12 +2078,12 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
@@ -2105,12 +2105,12 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2132,12 +2132,12 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2155,12 +2155,12 @@
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
+          <t>UTAH</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>UTAH</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
@@ -2182,12 +2182,12 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WISCONSIN</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>WISCONSIN</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
@@ -2209,12 +2209,12 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WYOMING</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>WYOMING</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2236,12 +2236,12 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WYOMING</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>WYOMING</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
@@ -2263,12 +2263,12 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>ALABAMA</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>ALABAMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2290,12 +2290,12 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>ARIZONA</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>ARIZONA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
@@ -2313,12 +2313,12 @@
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
@@ -2336,12 +2336,12 @@
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2359,12 +2359,12 @@
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2382,12 +2382,12 @@
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2405,12 +2405,12 @@
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
@@ -2428,12 +2428,12 @@
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
@@ -2451,12 +2451,12 @@
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
@@ -2474,12 +2474,12 @@
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2497,12 +2497,12 @@
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
@@ -2520,12 +2520,12 @@
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2543,12 +2543,12 @@
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
@@ -2566,12 +2566,12 @@
       <c r="B89" t="inlineStr"/>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
@@ -2589,12 +2589,12 @@
       <c r="B90" t="inlineStr"/>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
@@ -2612,12 +2612,12 @@
       <c r="B91" t="inlineStr"/>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E91" t="inlineStr">
@@ -2635,12 +2635,12 @@
       <c r="B92" t="inlineStr"/>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -2658,12 +2658,12 @@
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
@@ -2681,12 +2681,12 @@
       <c r="B94" t="inlineStr"/>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
@@ -2704,12 +2704,12 @@
       <c r="B95" t="inlineStr"/>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
@@ -2727,12 +2727,12 @@
       <c r="B96" t="inlineStr"/>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
@@ -2750,12 +2750,12 @@
       <c r="B97" t="inlineStr"/>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
@@ -2773,12 +2773,12 @@
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
@@ -2796,12 +2796,12 @@
       <c r="B99" t="inlineStr"/>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
@@ -2819,12 +2819,12 @@
       <c r="B100" t="inlineStr"/>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
@@ -2842,12 +2842,12 @@
       <c r="B101" t="inlineStr"/>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E101" t="inlineStr">
@@ -2865,12 +2865,12 @@
       <c r="B102" t="inlineStr"/>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
@@ -2888,12 +2888,12 @@
       <c r="B103" t="inlineStr"/>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -2911,12 +2911,12 @@
       <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -2934,12 +2934,12 @@
       <c r="B105" t="inlineStr"/>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>INDIANA</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>INDIANA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E105" t="inlineStr">
@@ -2957,12 +2957,12 @@
       <c r="B106" t="inlineStr"/>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>MAINE</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>MAINE</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E106" t="inlineStr">
@@ -2980,12 +2980,12 @@
       <c r="B107" t="inlineStr"/>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>NEW HAMPSHIRE</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>NEW HAMPSHIRE</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
@@ -3003,12 +3003,12 @@
       <c r="B108" t="inlineStr"/>
       <c r="C108" t="inlineStr">
         <is>
+          <t>NEW HAMPSHIRE</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D108" t="inlineStr">
-        <is>
-          <t>NEW HAMPSHIRE</t>
         </is>
       </c>
       <c r="E108" t="inlineStr">
@@ -3030,12 +3030,12 @@
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
         <is>
-          <t>OKLAHOMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E109" t="inlineStr">
@@ -3057,12 +3057,12 @@
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>SOUTH CAROLINA</t>
         </is>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>SOUTH CAROLINA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E110" t="inlineStr">
@@ -3084,12 +3084,12 @@
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TENNESSEE</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
         <is>
-          <t>TENNESSEE</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E111" t="inlineStr">
@@ -3111,12 +3111,12 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E112" t="inlineStr">
@@ -3138,12 +3138,12 @@
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -3165,12 +3165,12 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -3192,12 +3192,12 @@
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
@@ -3219,12 +3219,12 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
@@ -3246,12 +3246,12 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E117" t="inlineStr">
@@ -3273,12 +3273,12 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
@@ -3300,12 +3300,12 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
@@ -3327,12 +3327,12 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>VIRGINIA</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
         <is>
-          <t>VIRGINIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E120" t="inlineStr">
@@ -3354,12 +3354,12 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>VIRGINIA</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>VIRGINIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -3377,12 +3377,12 @@
       <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
@@ -3400,12 +3400,12 @@
       <c r="B123" t="inlineStr"/>
       <c r="C123" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -3423,12 +3423,12 @@
       <c r="B124" t="inlineStr"/>
       <c r="C124" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
@@ -3446,12 +3446,12 @@
       <c r="B125" t="inlineStr"/>
       <c r="C125" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
@@ -3469,12 +3469,12 @@
       <c r="B126" t="inlineStr"/>
       <c r="C126" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E126" t="inlineStr">
@@ -3492,12 +3492,12 @@
       <c r="B127" t="inlineStr"/>
       <c r="C127" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E127" t="inlineStr">
@@ -3515,12 +3515,12 @@
       <c r="B128" t="inlineStr"/>
       <c r="C128" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
@@ -3538,12 +3538,12 @@
       <c r="B129" t="inlineStr"/>
       <c r="C129" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
@@ -3561,12 +3561,12 @@
       <c r="B130" t="inlineStr"/>
       <c r="C130" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E130" t="inlineStr">
@@ -3584,12 +3584,12 @@
       <c r="B131" t="inlineStr"/>
       <c r="C131" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
@@ -3607,12 +3607,12 @@
       <c r="B132" t="inlineStr"/>
       <c r="C132" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
@@ -3630,12 +3630,12 @@
       <c r="B133" t="inlineStr"/>
       <c r="C133" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
@@ -3653,12 +3653,12 @@
       <c r="B134" t="inlineStr"/>
       <c r="C134" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
@@ -3676,12 +3676,12 @@
       <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E135" t="inlineStr">
@@ -3699,12 +3699,12 @@
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E136" t="inlineStr">
@@ -3722,12 +3722,12 @@
       <c r="B137" t="inlineStr"/>
       <c r="C137" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E137" t="inlineStr">
@@ -3745,12 +3745,12 @@
       <c r="B138" t="inlineStr"/>
       <c r="C138" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>GEORGIA</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
         <is>
-          <t>GEORGIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E138" t="inlineStr">
@@ -3768,12 +3768,12 @@
       <c r="B139" t="inlineStr"/>
       <c r="C139" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>LOUISIANA</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>LOUISIANA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
@@ -3791,12 +3791,12 @@
       <c r="B140" t="inlineStr"/>
       <c r="C140" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>MARYLAND</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>MARYLAND</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
@@ -3814,12 +3814,12 @@
       <c r="B141" t="inlineStr"/>
       <c r="C141" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>NEW YORK</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
         <is>
-          <t>NEW YORK</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E141" t="inlineStr">
@@ -3837,12 +3837,12 @@
       <c r="B142" t="inlineStr"/>
       <c r="C142" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OHIO</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>OHIO</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
@@ -3860,12 +3860,12 @@
       <c r="B143" t="inlineStr"/>
       <c r="C143" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>OKLAHOMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
@@ -3883,12 +3883,12 @@
       <c r="B144" t="inlineStr"/>
       <c r="C144" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OKLAHOMA</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>OKLAHOMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
@@ -3906,12 +3906,12 @@
       <c r="B145" t="inlineStr"/>
       <c r="C145" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>PENNSYLVANIA</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
         <is>
-          <t>PENNSYLVANIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E145" t="inlineStr">
@@ -3929,12 +3929,12 @@
       <c r="B146" t="inlineStr"/>
       <c r="C146" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TENNESSEE</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
         <is>
-          <t>TENNESSEE</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E146" t="inlineStr">
@@ -3952,12 +3952,12 @@
       <c r="B147" t="inlineStr"/>
       <c r="C147" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TENNESSEE</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
         <is>
-          <t>TENNESSEE</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E147" t="inlineStr">
@@ -3975,12 +3975,12 @@
       <c r="B148" t="inlineStr"/>
       <c r="C148" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
@@ -3998,12 +3998,12 @@
       <c r="B149" t="inlineStr"/>
       <c r="C149" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E149" t="inlineStr">
@@ -4021,12 +4021,12 @@
       <c r="B150" t="inlineStr"/>
       <c r="C150" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
@@ -4044,12 +4044,12 @@
       <c r="B151" t="inlineStr"/>
       <c r="C151" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
@@ -4067,12 +4067,12 @@
       <c r="B152" t="inlineStr"/>
       <c r="C152" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
@@ -4090,12 +4090,12 @@
       <c r="B153" t="inlineStr"/>
       <c r="C153" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WYOMING</t>
         </is>
       </c>
       <c r="D153" t="inlineStr">
         <is>
-          <t>WYOMING</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E153" t="inlineStr">
@@ -4113,12 +4113,12 @@
       <c r="B154" t="inlineStr"/>
       <c r="C154" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WYOMING</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>WYOMING</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
@@ -4136,12 +4136,12 @@
       <c r="B155" t="inlineStr"/>
       <c r="C155" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>ALABAMA</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>ALABAMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
@@ -4159,12 +4159,12 @@
       <c r="B156" t="inlineStr"/>
       <c r="C156" t="inlineStr">
         <is>
+          <t>FLORIDA</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D156" t="inlineStr">
-        <is>
-          <t>FLORIDA</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
@@ -4182,12 +4182,12 @@
       <c r="B157" t="inlineStr"/>
       <c r="C157" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>INDIANA</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>INDIANA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
@@ -4205,12 +4205,12 @@
       <c r="B158" t="inlineStr"/>
       <c r="C158" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>NEVADA</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>NEVADA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
@@ -4228,12 +4228,12 @@
       <c r="B159" t="inlineStr"/>
       <c r="C159" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OHIO</t>
         </is>
       </c>
       <c r="D159" t="inlineStr">
         <is>
-          <t>OHIO</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E159" t="inlineStr">
@@ -4251,12 +4251,12 @@
       <c r="B160" t="inlineStr"/>
       <c r="C160" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>OHIO</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>OHIO</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
@@ -4274,12 +4274,12 @@
       <c r="B161" t="inlineStr"/>
       <c r="C161" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>SOUTH DAKOTA</t>
         </is>
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>SOUTH DAKOTA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
@@ -4297,12 +4297,12 @@
       <c r="B162" t="inlineStr"/>
       <c r="C162" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D162" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E162" t="inlineStr">
@@ -4324,12 +4324,12 @@
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>ALABAMA</t>
         </is>
       </c>
       <c r="D163" t="inlineStr">
         <is>
-          <t>ALABAMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E163" t="inlineStr">
@@ -4351,12 +4351,12 @@
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>ALABAMA</t>
         </is>
       </c>
       <c r="D164" t="inlineStr">
         <is>
-          <t>ALABAMA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E164" t="inlineStr">
@@ -4374,12 +4374,12 @@
       <c r="B165" t="inlineStr"/>
       <c r="C165" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D165" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E165" t="inlineStr">
@@ -4397,12 +4397,12 @@
       <c r="B166" t="inlineStr"/>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D166" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E166" t="inlineStr">
@@ -4420,12 +4420,12 @@
       <c r="B167" t="inlineStr"/>
       <c r="C167" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D167" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E167" t="inlineStr">
@@ -4443,12 +4443,12 @@
       <c r="B168" t="inlineStr"/>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>LOUISIANA</t>
         </is>
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>LOUISIANA</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
@@ -4466,12 +4466,12 @@
       <c r="B169" t="inlineStr"/>
       <c r="C169" t="inlineStr">
         <is>
+          <t>MISSISSIPPI</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D169" t="inlineStr">
-        <is>
-          <t>MISSISSIPPI</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
@@ -4489,12 +4489,12 @@
       <c r="B170" t="inlineStr"/>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>NEW HAMPSHIRE</t>
         </is>
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>NEW HAMPSHIRE</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
@@ -4516,12 +4516,12 @@
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>SOUTH DAKOTA</t>
         </is>
       </c>
       <c r="D171" t="inlineStr">
         <is>
-          <t>SOUTH DAKOTA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E171" t="inlineStr">
@@ -4543,12 +4543,12 @@
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D172" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E172" t="inlineStr">
@@ -4570,12 +4570,12 @@
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>WISCONSIN</t>
         </is>
       </c>
       <c r="D173" t="inlineStr">
         <is>
-          <t>WISCONSIN</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E173" t="inlineStr">
@@ -4597,12 +4597,12 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>SOUTH CAROLINA</t>
         </is>
       </c>
       <c r="D174" t="inlineStr">
         <is>
-          <t>SOUTH CAROLINA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E174" t="inlineStr">
@@ -4624,12 +4624,12 @@
       </c>
       <c r="C175" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>TEXAS</t>
         </is>
       </c>
       <c r="D175" t="inlineStr">
         <is>
-          <t>TEXAS</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E175" t="inlineStr">
@@ -4651,12 +4651,12 @@
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>VIRGINIA</t>
         </is>
       </c>
       <c r="D176" t="inlineStr">
         <is>
-          <t>VIRGINIA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E176" t="inlineStr">
@@ -4678,12 +4678,12 @@
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>Municipality</t>
+          <t>MAINE</t>
         </is>
       </c>
       <c r="D177" t="inlineStr">
         <is>
-          <t>MAINE</t>
+          <t>Municipality</t>
         </is>
       </c>
       <c r="E177" t="inlineStr">
@@ -4705,12 +4705,12 @@
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>County</t>
+          <t>FLORIDA</t>
         </is>
       </c>
       <c r="D178" t="inlineStr">
         <is>
-          <t>FLORIDA</t>
+          <t>County</t>
         </is>
       </c>
       <c r="E178" t="inlineStr">
@@ -4728,12 +4728,12 @@
       <c r="B179" t="inlineStr"/>
       <c r="C179" t="inlineStr">
         <is>
+          <t>TEXAS</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
           <t>State Agency</t>
-        </is>
-      </c>
-      <c r="D179" t="inlineStr">
-        <is>
-          <t>TEXAS</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">

</xml_diff>